<commit_message>
BP Voorstel bijgewerkt op basis van feedback promotor
</commit_message>
<xml_diff>
--- a/Tijdsregistratie.xlsx
+++ b/Tijdsregistratie.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hogent-my.sharepoint.com/personal/stijn_coppens_student_hogent_be/Documents/2023/Bachelorproef/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="8_{C65F7E1B-A6BE-426F-9CFF-D1DC12FB3089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A1F6301-DE42-45B5-93E6-D038D8BB705C}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{C65F7E1B-A6BE-426F-9CFF-D1DC12FB3089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB43EAF-D284-4162-BE38-A61E4AFDACF3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{2B11156B-3A53-4B26-8968-BA2F706718BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{2B11156B-3A53-4B26-8968-BA2F706718BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="4" r:id="rId2"/>
     <sheet name="07022024" sheetId="1" r:id="rId3"/>
     <sheet name="08022024" sheetId="3" r:id="rId4"/>
+    <sheet name="09022024" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="122">
   <si>
     <t>Datum</t>
   </si>
@@ -306,6 +329,105 @@
   </si>
   <si>
     <t>chh B 193 pc04</t>
+  </si>
+  <si>
+    <t>mkh B 57 we04c021</t>
+  </si>
+  <si>
+    <t>chh B 209 re22c137 ug-gdbc0x2</t>
+  </si>
+  <si>
+    <t>rmhost B 72 beid</t>
+  </si>
+  <si>
+    <t>rmhost B 72 bramtop</t>
+  </si>
+  <si>
+    <t>rmhost B 72 egel</t>
+  </si>
+  <si>
+    <t>rmhost B 73 gaudin</t>
+  </si>
+  <si>
+    <t>rmhost B 72 ilta</t>
+  </si>
+  <si>
+    <t>rmhost B 72 koru</t>
+  </si>
+  <si>
+    <t>rmhost B 72 lete</t>
+  </si>
+  <si>
+    <t>rmhost B 72 captain</t>
+  </si>
+  <si>
+    <t>rmhost B 73 meramobi</t>
+  </si>
+  <si>
+    <t>rmhost B 72 miho</t>
+  </si>
+  <si>
+    <t>rmhost B 73 nelson</t>
+  </si>
+  <si>
+    <t>rmhost B 72 rch05</t>
+  </si>
+  <si>
+    <t>rmhost B 72 sakkee</t>
+  </si>
+  <si>
+    <t>rmhost B 72 trump</t>
+  </si>
+  <si>
+    <t>rmhost B 73 we05c027</t>
+  </si>
+  <si>
+    <t>rmhost B 72 we05g004</t>
+  </si>
+  <si>
+    <t>pagina</t>
+  </si>
+  <si>
+    <t>07022024</t>
+  </si>
+  <si>
+    <t>rmhost B 72 lucca</t>
+  </si>
+  <si>
+    <t>rmhost B 73 vm201</t>
+  </si>
+  <si>
+    <t>rmhost B 73 meccano</t>
+  </si>
+  <si>
+    <t>rmhost N 53 mongofarmdev</t>
+  </si>
+  <si>
+    <t>rmhost B 73 quigon</t>
+  </si>
+  <si>
+    <t>rmhost B 73 cthulhu</t>
+  </si>
+  <si>
+    <t>mkh N 20 ea06c154</t>
+  </si>
+  <si>
+    <t>rmhost B 72 aussie</t>
+  </si>
+  <si>
+    <t>mkh B 91 we06c221</t>
+  </si>
+  <si>
+    <t>mkh B 91 we06c222</t>
+  </si>
+  <si>
+    <t>mkh   clsh2709001</t>
+  </si>
+  <si>
+    <t>mkh   clsh1510001</t>
+  </si>
+  <si>
+    <t>Te weinig info in aanvraag om locatie terug te vinden, mail verzonden</t>
   </si>
 </sst>
 </file>
@@ -314,7 +436,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ am/pm"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -362,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,14 +499,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -396,7 +532,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -413,7 +549,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -430,7 +566,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -471,7 +624,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -494,35 +647,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5B5F6CD-8ACE-4E45-8B01-474BA05E36A6}" name="Table2" displayName="Table2" ref="A1:J3" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:J3" xr:uid="{E5B5F6CD-8ACE-4E45-8B01-474BA05E36A6}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D78D2B78-ABE0-4C9F-AB45-D50B0E032C81}" name="Datum" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F95525B3-F970-4D18-A087-BFF197A681F0}" name="Aantal toevoegingen" dataDxfId="23">
-      <calculatedColumnFormula>'08022024'!J5</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5B5F6CD-8ACE-4E45-8B01-474BA05E36A6}" name="Table2" displayName="Table2" ref="A1:K14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:K14" xr:uid="{E5B5F6CD-8ACE-4E45-8B01-474BA05E36A6}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{D78D2B78-ABE0-4C9F-AB45-D50B0E032C81}" name="Datum" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{A0FCC866-D19A-4F98-A878-53A624EE44F9}" name="pagina" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F95525B3-F970-4D18-A087-BFF197A681F0}" name="Aantal toevoegingen" dataDxfId="29">
+      <calculatedColumnFormula array="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{25727468-A7AC-4814-A38A-F4F31CA93F5F}" name="Tijdsduur voor toevoeging" dataDxfId="22">
+    <tableColumn id="3" xr3:uid="{25727468-A7AC-4814-A38A-F4F31CA93F5F}" name="Tijdsduur voor toevoeging" dataDxfId="28">
       <calculatedColumnFormula>'07022024'!K5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2A8BD552-F257-4DFE-A3F3-61C735897D2F}" name="Aantal wijzigingen" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{2A8BD552-F257-4DFE-A3F3-61C735897D2F}" name="Aantal wijzigingen" dataDxfId="27">
       <calculatedColumnFormula>'08022024'!J6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7B7753AD-A315-4D3F-B0A1-30AC7CBFBF1B}" name="Tijdsduur voor wijziging" dataDxfId="20">
+    <tableColumn id="5" xr3:uid="{7B7753AD-A315-4D3F-B0A1-30AC7CBFBF1B}" name="Tijdsduur voor wijziging" dataDxfId="26">
       <calculatedColumnFormula>'08022024'!K5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D625FED6-A7E3-4D71-9546-ABADB957BBB4}" name="Aantal verwijderingen" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{D625FED6-A7E3-4D71-9546-ABADB957BBB4}" name="Aantal verwijderingen" dataDxfId="25">
       <calculatedColumnFormula>'07022024'!J7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7A9AD3D5-10FE-4949-955B-E8F2D5547F04}" name="Tijdsduur voor verwijderen" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{7A9AD3D5-10FE-4949-955B-E8F2D5547F04}" name="Tijdsduur voor verwijderen" dataDxfId="24">
       <calculatedColumnFormula>'07022024'!K7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B66100FA-467D-44B8-86F2-E8EE6C78E6D7}" name="Tijdsduur updates" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{B66100FA-467D-44B8-86F2-E8EE6C78E6D7}" name="Tijdsduur updates" dataDxfId="23">
       <calculatedColumnFormula>'07022024'!K8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{608BB356-C6D5-4A54-82AF-433FB5604410}" name="Totaal aantal verwerkte aanvragen" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{608BB356-C6D5-4A54-82AF-433FB5604410}" name="Totaal aantal verwerkte aanvragen" dataDxfId="22">
       <calculatedColumnFormula>'07022024'!J9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{BADA0CE9-E5D4-4556-B230-1C87E7357A3A}" name="Totaal tijdsduur" dataDxfId="15">
+    <tableColumn id="10" xr3:uid="{BADA0CE9-E5D4-4556-B230-1C87E7357A3A}" name="Totaal tijdsduur" dataDxfId="21">
       <calculatedColumnFormula>'07022024'!K9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -531,17 +685,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE7BDC3D-39E6-48BA-9C89-45C7D5EF874F}" name="Table145" displayName="Table145" ref="A1:F28" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE7BDC3D-39E6-48BA-9C89-45C7D5EF874F}" name="Table145" displayName="Table145" ref="A1:F28" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:F28" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1B3A7ABB-C371-4A45-9D2D-B19C89F85E2F}" name="Datum" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{1B3A7ABB-C371-4A45-9D2D-B19C89F85E2F}" name="Datum" dataDxfId="19">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CDA06A3E-15DF-45A5-8BCF-D4AA44DF6789}" name="Actie" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{CDA06A3E-15DF-45A5-8BCF-D4AA44DF6789}" name="Actie" dataDxfId="18">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("mkh ",C2)),"ADD",IF(ISNUMBER(SEARCH("chh ",C2)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C2)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C2)),"UPDATE",""))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9293EEFE-FF0E-4252-9E8F-CEAC7F06C8F0}" name="Command" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{D4C11C17-9153-45C4-9580-7FDF4B628FE5}" name="Tijdsduur" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{9293EEFE-FF0E-4252-9E8F-CEAC7F06C8F0}" name="Command" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{D4C11C17-9153-45C4-9580-7FDF4B628FE5}" name="Tijdsduur" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{C151002B-3F02-4C8F-9EBC-A004DFEAE77E}" name="Opmerking1"/>
     <tableColumn id="6" xr3:uid="{9C5D85F2-B743-4407-AFDC-880181162DBA}" name="Opmerking2"/>
   </tableColumns>
@@ -550,15 +704,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:F28" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{95C1020F-166E-4B9A-A951-EA488AD5B306}" name="Datum" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{95C1020F-166E-4B9A-A951-EA488AD5B306}" name="Datum" dataDxfId="14">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{84E2B627-9135-4186-B3FA-0CD80BBB65AA}" name="Actie" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{43661A0F-4FB9-4AE8-B041-461E20DB2B34}" name="Command" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4CB1C556-821A-4D72-8A46-DBF71D0CF28A}" name="Tijdsduur" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{84E2B627-9135-4186-B3FA-0CD80BBB65AA}" name="Actie" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{43661A0F-4FB9-4AE8-B041-461E20DB2B34}" name="Command" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{4CB1C556-821A-4D72-8A46-DBF71D0CF28A}" name="Tijdsduur" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{D2D3AFCA-8F37-493F-8304-EE9CF40A8EBE}" name="Opmerking1"/>
     <tableColumn id="6" xr3:uid="{14451886-1FBC-4EDF-B567-2FDBF09FBA2D}" name="Opmerking2"/>
   </tableColumns>
@@ -567,17 +721,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A906162-8C55-4D31-8B74-6EBBA6FFBA2A}" name="Table14" displayName="Table14" ref="A1:F31" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A906162-8C55-4D31-8B74-6EBBA6FFBA2A}" name="Table14" displayName="Table14" ref="A1:F31" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:F31" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B4752309-6451-4960-A216-BB6F71F3E539}" name="Datum" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C2CBEBD3-269C-4ECE-B9CB-2068D2DF0AA0}" name="Actie" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{B4752309-6451-4960-A216-BB6F71F3E539}" name="Datum" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C2CBEBD3-269C-4ECE-B9CB-2068D2DF0AA0}" name="Actie" dataDxfId="8">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("mkh ",C2)),"ADD",IF(ISNUMBER(SEARCH("chh ",C2)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C2)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C2)),"UPDATE",""))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{83213F11-B23A-4630-98D4-2BB4775D64B0}" name="Command" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1F0D4896-8A4A-4A01-BFC4-5CB0C789920E}" name="Tijdsduur" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{83213F11-B23A-4630-98D4-2BB4775D64B0}" name="Command" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1F0D4896-8A4A-4A01-BFC4-5CB0C789920E}" name="Tijdsduur" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{7A98BE10-2779-44FD-A6F6-F4BB90B97F77}" name="Opmerking1"/>
     <tableColumn id="6" xr3:uid="{258825D9-DB74-41AE-99F4-B6C0CD8864EB}" name="Opmerking2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58EE1D1B-A953-4F85-B12D-8CF6A08C9740}" name="Table1456" displayName="Table1456" ref="A1:F28" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F28" xr:uid="{9BE52DD0-0866-4682-8AA0-7D0A8298E126}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2E13FE21-D7F6-4B2F-8FB3-83E062DE7D4D}" name="Datum" dataDxfId="4">
+      <calculatedColumnFormula>NOW()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{8D46EBA2-7343-40CD-8B43-A18828C14D42}" name="Actie" dataDxfId="3">
+      <calculatedColumnFormula>IF(ISNUMBER(SEARCH("mkh ",C2)),"ADD",IF(ISNUMBER(SEARCH("chh ",C2)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C2)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C2)),"UPDATE",""))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{603954BB-4990-4FCB-87DC-083EE7BE5364}" name="Command" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3A05C20B-6B50-4827-A08E-1C3E0FBE0735}" name="Tijdsduur" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{0FD6DAD9-3100-4C6B-BDDD-60D07BD62E90}" name="Opmerking1"/>
+    <tableColumn id="6" xr3:uid="{4F67BB6A-E87F-4BF2-8536-A8F292E8EF4E}" name="Opmerking2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -880,138 +1053,644 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259A3E81-D374-4272-9D7D-868849FCFAE7}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.08984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="31.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45329</v>
       </c>
-      <c r="B2" s="1">
-        <f>'07022024'!J5</f>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="1" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
         <v>3</v>
       </c>
-      <c r="C2" s="4">
-        <f>'07022024'!K5</f>
+      <c r="D2" s="10" cm="1">
+        <f t="array" aca="1" ref="D2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
         <v>4.6296296296296294E-3</v>
       </c>
-      <c r="D2" s="1">
-        <f>'07022024'!J6</f>
+      <c r="E2" s="1" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
         <v>5</v>
       </c>
-      <c r="E2" s="4">
-        <f>'08022024'!K5</f>
-        <v>9.8379629629629615E-3</v>
-      </c>
-      <c r="F2" s="1">
-        <f>'07022024'!J7</f>
+      <c r="F2" s="10" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>3.6689814814814814E-3</v>
+      </c>
+      <c r="G2" s="1" cm="1">
+        <f t="array" aca="1" ref="G2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
         <v>18</v>
       </c>
-      <c r="G2" s="4">
-        <f>'07022024'!K7</f>
+      <c r="H2" s="10" cm="1">
+        <f t="array" aca="1" ref="H2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
         <v>3.7500000000000003E-3</v>
       </c>
-      <c r="H2" s="4">
-        <f>'07022024'!K8</f>
+      <c r="I2" s="10" cm="1">
+        <f t="array" aca="1" ref="I2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
         <v>2.9861111111111113E-3</v>
       </c>
-      <c r="I2" s="1">
-        <f>'07022024'!J9</f>
+      <c r="J2" s="1" cm="1">
+        <f t="array" aca="1" ref="J2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
         <v>26</v>
       </c>
-      <c r="J2" s="4">
-        <f>'07022024'!K9</f>
+      <c r="K2" s="10" cm="1">
+        <f t="array" aca="1" ref="K2" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
         <v>1.5034722222222222E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45330</v>
       </c>
-      <c r="B3" s="1">
-        <f>'08022024'!J5</f>
+      <c r="B3" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>08022024</v>
+      </c>
+      <c r="C3" s="8" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
         <v>16</v>
       </c>
-      <c r="C3" s="4">
-        <f>'08022024'!K5</f>
+      <c r="D3" s="10" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
         <v>9.8379629629629615E-3</v>
       </c>
-      <c r="D3" s="1">
-        <f>'08022024'!J6</f>
+      <c r="E3" s="1" cm="1">
+        <f t="array" aca="1" ref="E3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
         <v>13</v>
       </c>
-      <c r="E3" s="4">
-        <f>'08022024'!K6</f>
+      <c r="F3" s="10" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
         <v>5.9143518518518529E-3</v>
       </c>
-      <c r="F3" s="1">
-        <f>'08022024'!J7</f>
+      <c r="G3" s="1" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
         <v>0</v>
       </c>
-      <c r="G3" s="4">
-        <f>'08022024'!K7</f>
+      <c r="H3" s="10" cm="1">
+        <f t="array" aca="1" ref="H3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
         <v>0</v>
       </c>
-      <c r="H3" s="4">
-        <f>'08022024'!K8</f>
+      <c r="I3" s="10" cm="1">
+        <f t="array" aca="1" ref="I3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
         <v>1.8055555555555557E-3</v>
       </c>
-      <c r="I3" s="1">
-        <f>'08022024'!J9</f>
+      <c r="J3" s="1" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
         <v>30</v>
       </c>
-      <c r="J3" s="4">
-        <f>'08022024'!K9</f>
+      <c r="K3" s="10" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
         <v>1.7557870370370373E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>09022024</v>
+      </c>
+      <c r="C4" s="8" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>1.0995370370370371E-3</v>
+      </c>
+      <c r="E4" s="1" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="G4" s="1" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>23</v>
+      </c>
+      <c r="H4" s="10" cm="1">
+        <f t="array" aca="1" ref="H4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>4.7337962962962958E-3</v>
+      </c>
+      <c r="I4" s="10" cm="1">
+        <f t="array" aca="1" ref="I4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" cm="1">
+        <f t="array" aca="1" ref="J4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>27</v>
+      </c>
+      <c r="K4" s="10" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>6.1805555555555555E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45334</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>12022024</v>
+      </c>
+      <c r="C5" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D5" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F5" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G5" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H5" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I5" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J5" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K5" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45335</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>13022024</v>
+      </c>
+      <c r="C6" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D6" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F6" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G6" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H6" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I6" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J6" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K6" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45336</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>14022024</v>
+      </c>
+      <c r="C7" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D7" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F7" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G7" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H7" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I7" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J7" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K7" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K7" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45337</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>15022024</v>
+      </c>
+      <c r="C8" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D8" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E8" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F8" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G8" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H8" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I8" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J8" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K8" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K8" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45338</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>16022024</v>
+      </c>
+      <c r="C9" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D9" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F9" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K9" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45341</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>19022024</v>
+      </c>
+      <c r="C10" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D10" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F10" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G10" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H10" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K10" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K10" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45342</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>20022024</v>
+      </c>
+      <c r="C11" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D11" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F11" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G11" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H11" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K11" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45343</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>21022024</v>
+      </c>
+      <c r="C12" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D12" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E12" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F12" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G12" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H12" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I12" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J12" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K12" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K12" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45344</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>22022024</v>
+      </c>
+      <c r="C13" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D13" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E13" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F13" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K13" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K13" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45345</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>TEXT(Table2[[#This Row],[Datum]],"ddmmyyyy")</f>
+        <v>23022024</v>
+      </c>
+      <c r="C14" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="D14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K5")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="E14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F14" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="F14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k6")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G14" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="G14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H14" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="H14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K7")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I14" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="I14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!K8")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="J14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!J9")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K14" s="10" t="e" cm="1">
+        <f t="array" aca="1" ref="K14" ca="1">INDIRECT("'" &amp; Table2[[#This Row],[pagina]] &amp; "'!k9")</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -1027,25 +1706,25 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,10 +1747,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f ca="1">NOW()</f>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B2" s="1" t="str">
         <f t="shared" ref="B2:B28" si="0">IF(ISNUMBER(SEARCH("mkh ",C2)),"ADD",IF(ISNUMBER(SEARCH("chh ",C2)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C2)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C2)),"UPDATE",""))))</f>
@@ -1093,10 +1772,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A28" ca="1" si="1">NOW()</f>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1115,10 +1794,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1143,10 +1822,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1159,7 +1838,8 @@
         <v>5.2083333333333333E-4</v>
       </c>
       <c r="H5" s="2">
-        <v>45329</v>
+        <f ca="1">$A$2</f>
+        <v>45331.633002893519</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -1170,13 +1850,13 @@
       </c>
       <c r="K5" s="4">
         <f ca="1">SUMIFS(Table145[Tijdsduur],Table145[Datum],H5,Table145[Actie],I5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.9675925925925924E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1192,7 +1872,8 @@
         <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>45329</v>
+        <f t="shared" ref="H6:H9" ca="1" si="2">$A$2</f>
+        <v>45331.633002893519</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -1203,13 +1884,13 @@
       </c>
       <c r="K6" s="4">
         <f ca="1">SUMIFS(Table145[Tijdsduur],Table145[Datum],H6,Table145[Actie],I6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3.6689814814814814E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1222,7 +1903,8 @@
         <v>3.7037037037037035E-4</v>
       </c>
       <c r="H7" s="2">
-        <v>45329</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>42</v>
@@ -1233,13 +1915,13 @@
       </c>
       <c r="K7" s="4">
         <f ca="1">SUMIFS(Table145[Tijdsduur],Table145[Datum],H7,Table145[Actie],I7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3.7500000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1252,7 +1934,8 @@
         <v>3.1250000000000001E-4</v>
       </c>
       <c r="H8" s="2">
-        <v>45329</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>41</v>
@@ -1263,13 +1946,13 @@
       </c>
       <c r="K8" s="4">
         <f ca="1">SUMIFS(Table145[Tijdsduur],Table145[Datum],H8,Table145[Actie],I8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2.9861111111111113E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1282,7 +1965,8 @@
         <v>1.9675925925925926E-4</v>
       </c>
       <c r="H9" s="2">
-        <v>45329</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>43</v>
@@ -1293,13 +1977,13 @@
       </c>
       <c r="K9" s="4">
         <f ca="1">SUM(K5:K8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1.2372685185185184E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1312,10 +1996,10 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1328,10 +2012,10 @@
         <v>2.4305555555555552E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1344,10 +2028,10 @@
         <v>1.6203703703703703E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1360,10 +2044,10 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1376,10 +2060,10 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1392,10 +2076,10 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1408,10 +2092,10 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1424,10 +2108,10 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1440,10 +2124,10 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1456,10 +2140,10 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1472,10 +2156,10 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1488,10 +2172,10 @@
         <v>1.8518518518518518E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1504,10 +2188,10 @@
         <v>1.7361111111111112E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1520,10 +2204,10 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1536,10 +2220,10 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1552,10 +2236,10 @@
         <v>1.8518518518518518E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1571,10 +2255,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1593,10 +2277,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45330.83291203704</v>
+        <v>45331.633002893519</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1609,14 +2293,14 @@
         <v>2.9861111111111113E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="str">
         <f>IF(ISNUMBER(SEARCH("mkh ",C29)),"ADD",IF(ISNUMBER(SEARCH("chh ",C29)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C29)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C29)),"UPDATE",""))))</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="str">
         <f>IF(ISNUMBER(SEARCH("mkh ",C30)),"ADD",IF(ISNUMBER(SEARCH("chh ",C30)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C30)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C30)),"UPDATE",""))))</f>
@@ -1640,21 +2324,21 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1677,7 +2361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45329</v>
       </c>
@@ -1700,7 +2384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45329</v>
       </c>
@@ -1720,7 +2404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45329</v>
       </c>
@@ -1746,7 +2430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45329</v>
       </c>
@@ -1774,7 +2458,7 @@
         <v>4.6296296296296294E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45329</v>
       </c>
@@ -1805,7 +2489,7 @@
         <v>3.6689814814814814E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45329</v>
       </c>
@@ -1833,7 +2517,7 @@
         <v>3.7500000000000003E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45329</v>
       </c>
@@ -1861,7 +2545,7 @@
         <v>2.9861111111111113E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45329</v>
       </c>
@@ -1889,7 +2573,7 @@
         <v>1.5034722222222222E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45329</v>
       </c>
@@ -1903,7 +2587,7 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45329</v>
       </c>
@@ -1917,7 +2601,7 @@
         <v>2.4305555555555552E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45329</v>
       </c>
@@ -1931,7 +2615,7 @@
         <v>1.6203703703703703E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45329</v>
       </c>
@@ -1945,7 +2629,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45329</v>
       </c>
@@ -1959,7 +2643,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45329</v>
       </c>
@@ -1973,7 +2657,7 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45329</v>
       </c>
@@ -1987,7 +2671,7 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45329</v>
       </c>
@@ -2001,7 +2685,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45329</v>
       </c>
@@ -2015,7 +2699,7 @@
         <v>2.199074074074074E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45329</v>
       </c>
@@ -2029,7 +2713,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45329</v>
       </c>
@@ -2043,7 +2727,7 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45329</v>
       </c>
@@ -2057,7 +2741,7 @@
         <v>1.8518518518518518E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45329</v>
       </c>
@@ -2071,7 +2755,7 @@
         <v>1.7361111111111112E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45329</v>
       </c>
@@ -2085,7 +2769,7 @@
         <v>1.9675925925925926E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45329</v>
       </c>
@@ -2099,7 +2783,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45329</v>
       </c>
@@ -2113,7 +2797,7 @@
         <v>1.8518518518518518E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45329</v>
       </c>
@@ -2130,7 +2814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45329</v>
       </c>
@@ -2150,7 +2834,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45329</v>
       </c>
@@ -2164,14 +2848,14 @@
         <v>2.9861111111111113E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="str">
         <f t="shared" ref="B29:B30" si="0">IF(ISNUMBER(SEARCH("mkh ",C29)),"ADD",IF(ISNUMBER(SEARCH("chh ",C29)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C29)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C29)),"UPDATE",""))))</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2191,26 +2875,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FB24C5-0C28-4D64-B019-3A6C16F9B1D6}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2233,7 +2917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45330</v>
       </c>
@@ -2251,7 +2935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45330</v>
       </c>
@@ -2266,7 +2950,7 @@
         <v>4.9768518518518521E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45330</v>
       </c>
@@ -2293,7 +2977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45330</v>
       </c>
@@ -2323,7 +3007,7 @@
         <v>9.8379629629629615E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45330</v>
       </c>
@@ -2353,7 +3037,7 @@
         <v>5.9143518518518529E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45330</v>
       </c>
@@ -2386,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45330</v>
       </c>
@@ -2416,7 +3100,7 @@
         <v>1.8055555555555557E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45330</v>
       </c>
@@ -2446,7 +3130,7 @@
         <v>1.7557870370370373E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45330</v>
       </c>
@@ -2461,7 +3145,7 @@
         <v>3.7037037037037035E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45330</v>
       </c>
@@ -2476,7 +3160,7 @@
         <v>3.9351851851851852E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45330</v>
       </c>
@@ -2491,7 +3175,7 @@
         <v>3.7037037037037035E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45330</v>
       </c>
@@ -2506,7 +3190,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45330</v>
       </c>
@@ -2521,7 +3205,7 @@
         <v>3.8194444444444446E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45330</v>
       </c>
@@ -2539,7 +3223,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45330</v>
       </c>
@@ -2557,7 +3241,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45330</v>
       </c>
@@ -2575,7 +3259,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45330</v>
       </c>
@@ -2590,7 +3274,7 @@
         <v>4.0509259259259258E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45330</v>
       </c>
@@ -2605,7 +3289,7 @@
         <v>4.2824074074074075E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45330</v>
       </c>
@@ -2620,7 +3304,7 @@
         <v>4.0509259259259258E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45330</v>
       </c>
@@ -2635,7 +3319,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45330</v>
       </c>
@@ -2650,7 +3334,7 @@
         <v>3.3564814814814812E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45330</v>
       </c>
@@ -2665,7 +3349,7 @@
         <v>3.5879629629629635E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45330</v>
       </c>
@@ -2680,7 +3364,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45330</v>
       </c>
@@ -2695,7 +3379,7 @@
         <v>3.3564814814814812E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45330</v>
       </c>
@@ -2710,7 +3394,7 @@
         <v>3.0092592592592595E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45330</v>
       </c>
@@ -2725,7 +3409,7 @@
         <v>3.5879629629629635E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45330</v>
       </c>
@@ -2746,7 +3430,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45330</v>
       </c>
@@ -2764,7 +3448,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45330</v>
       </c>
@@ -2779,7 +3463,7 @@
         <v>4.1666666666666669E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45330</v>
       </c>
@@ -2794,8 +3478,8 @@
         <v>1.8055555555555557E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="str">
         <f>IF(ISNUMBER(SEARCH("mkh ",C32)),"ADD",IF(ISNUMBER(SEARCH("chh ",C32)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C32)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C32)),"UPDATE",""))))</f>
         <v/>
@@ -2810,4 +3494,621 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0047CC-CED0-4097-877D-8107E4973DF1}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <f ca="1">NOW()</f>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f t="shared" ref="B2:B28" si="0">IF(ISNUMBER(SEARCH("mkh ",C2)),"ADD",IF(ISNUMBER(SEARCH("chh ",C2)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C2)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C2)),"UPDATE",""))))</f>
+        <v>ADD</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4">
+        <v>4.9768518518518521E-4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A28" ca="1" si="1">NOW()</f>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CHANGE</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.4722222222222224E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.6620370370370372E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <f ca="1">$A$2</f>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <f>COUNTIF(Table1456[Actie],I5)</f>
+        <v>3</v>
+      </c>
+      <c r="K5" s="4">
+        <f ca="1">SUMIFS(Table1456[Tijdsduur],Table1456[Datum],H5,Table1456[Actie],I5)</f>
+        <v>1.0995370370370371E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.8518518518518518E-4</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H9" ca="1" si="2">$A$2</f>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1">
+        <f>COUNTIF(Table1456[Actie],I6)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <f ca="1">SUMIFS(Table1456[Tijdsduur],Table1456[Datum],H6,Table1456[Actie],I6)</f>
+        <v>3.4722222222222224E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1">
+        <f>COUNTIF(Table1456[Actie],I7)</f>
+        <v>23</v>
+      </c>
+      <c r="K7" s="4">
+        <f ca="1">SUMIFS(Table1456[Tijdsduur],Table1456[Datum],H7,Table1456[Actie],I7)</f>
+        <v>4.7337962962962958E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="1">
+        <f>COUNTIF(Table1456[Actie],I8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <f ca="1">SUMIFS(Table1456[Tijdsduur],Table1456[Datum],H8,Table1456[Actie],I8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1">
+        <f>SUM(J5:J8)</f>
+        <v>27</v>
+      </c>
+      <c r="K9" s="4">
+        <f ca="1">SUM(K5:K8)</f>
+        <v>6.1805555555555555E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.8518518518518518E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.199074074074074E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.199074074074074E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.8518518518518518E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.199074074074074E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.4305555555555552E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.8518518518518518E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3.1250000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.7361111111111112E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.8518518518518518E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.9675925925925926E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.6203703703703703E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ADD</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3.2407407407407406E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>REMOVE</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.199074074074074E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>45331.633002893519</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ADD</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2.7777777777777778E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1" t="str">
+        <f>IF(ISNUMBER(SEARCH("mkh ",C29)),"ADD",IF(ISNUMBER(SEARCH("chh ",C29)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C29)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C29)),"UPDATE",""))))</f>
+        <v>ADD</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3.1250000000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="1" t="str">
+        <f>IF(ISNUMBER(SEARCH("mkh ",C30)),"ADD",IF(ISNUMBER(SEARCH("chh ",C30)),"CHANGE",IF(ISNUMBER(SEARCH("rmhost ",C30)),"REMOVE",IF(ISNUMBER(SEARCH("Update",C30)),"UPDATE",""))))</f>
+        <v>ADD</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="4">
+        <v>8.564814814814815E-4</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.689814814814815E-3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>